<commit_message>
Agregar ejemplos de productos y categorías activos e inactivos en plantillas Excel
- Agregar ejemplo de producto activo (Filtro HEPA H13)
- Agregar ejemplo de producto inactivo (Filtro Prefiltro G4)
- Agregar ejemplo de categoría activa (Filtros HEPA)
- Agregar ejemplo de categoría inactiva (Filtros Descontinuados)
- Regenerar plantillas Excel con los nuevos ejemplos
</commit_message>
<xml_diff>
--- a/public/templates/categorias-template.xlsx
+++ b/public/templates/categorias-template.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -442,9 +442,29 @@
         <v>active</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Filtros Descontinuados</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Discontinued Filters</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Categoría de filtros que ya no se fabrican</v>
+      </c>
+      <c r="D3" t="str">
+        <v>Category of filters that are no longer manufactured</v>
+      </c>
+      <c r="E3" t="str">
+        <v/>
+      </c>
+      <c r="F3" t="str">
+        <v>inactive</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>